<commit_message>
Plans page 20 Cases Done
</commit_message>
<xml_diff>
--- a/verizonWireless/src/main/java/resources/VerizonWireless_Planspage_Elements.xlsx
+++ b/verizonWireless/src/main/java/resources/VerizonWireless_Planspage_Elements.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\IdeaProjects\AutomationFramework_Team3\verizonWireless\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3B31AB-19EA-4966-B4A7-44424C8B4D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C275CECC-B4A2-40F3-98C9-017A8475A1F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="2415" windowWidth="2400" windowHeight="585" activeTab="2" xr2:uid="{9A919245-3C8B-46DA-92D6-7A0DBF9692D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{9A919245-3C8B-46DA-92D6-7A0DBF9692D7}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanspageURL" sheetId="1" r:id="rId1"/>
     <sheet name="PlansDropDown" sheetId="2" r:id="rId2"/>
     <sheet name="PlanDeals" sheetId="3" r:id="rId3"/>
+    <sheet name="PhonesDropDown" sheetId="5" r:id="rId4"/>
+    <sheet name="FeaturedPhones" sheetId="6" r:id="rId5"/>
+    <sheet name="AppsAndServicesList" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>https://www.verizon.com/plans/</t>
   </si>
@@ -78,6 +81,93 @@
   </si>
   <si>
     <t>YouTube TV</t>
+  </si>
+  <si>
+    <t>Smartphones</t>
+  </si>
+  <si>
+    <t>Trade in your phone</t>
+  </si>
+  <si>
+    <t>Basic phones</t>
+  </si>
+  <si>
+    <t>Certified pre-owned</t>
+  </si>
+  <si>
+    <t>Prepaid phones</t>
+  </si>
+  <si>
+    <t>Bring your own device</t>
+  </si>
+  <si>
+    <t>Unlocked phones</t>
+  </si>
+  <si>
+    <t>Phone accessories</t>
+  </si>
+  <si>
+    <t>Apple iPhone SE (2020)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 Pro</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 Pro Max</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S20 5G UW</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S20+ 5G</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A51</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Note 10+</t>
+  </si>
+  <si>
+    <t>Google Pixel 4</t>
+  </si>
+  <si>
+    <t>Moto Razr</t>
+  </si>
+  <si>
+    <t>OnePlus 8 5G UW</t>
+  </si>
+  <si>
+    <t>motorola edge+</t>
+  </si>
+  <si>
+    <t>My Verizon</t>
+  </si>
+  <si>
+    <t>Verizon Cloud</t>
+  </si>
+  <si>
+    <t>Smart Family</t>
+  </si>
+  <si>
+    <t>Device trade-in</t>
+  </si>
+  <si>
+    <t>Device Protection</t>
+  </si>
+  <si>
+    <t>Call Filter</t>
+  </si>
+  <si>
+    <t>Premium Visual Voicemail</t>
+  </si>
+  <si>
+    <t>Hum</t>
+  </si>
+  <si>
+    <t>See More Apps</t>
   </si>
 </sst>
 </file>
@@ -529,7 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3187884-C037-479B-A206-35A503309E4A}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -561,4 +651,208 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA295873-55CE-4DFA-B510-A17318EA3E6E}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1620329-B999-48D1-8F32-B2CBFCF4A833}">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AC67A1-6746-4139-9205-01020DA2BCC2}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>